<commit_message>
mejorando controlador, leyendo por filas el csv
</commit_message>
<xml_diff>
--- a/public/files/csv/plantilla.xlsx
+++ b/public/files/csv/plantilla.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XAMPP\htdocs\SistemaGestionDocumental\public\files\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1567ECBE-A6A9-4A93-9689-248A843B79DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E6DE49-A7EC-48F2-B7A1-BEAE6E9931A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{E1F0702F-A2B5-47DB-BA00-427920F7F315}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E1F0702F-A2B5-47DB-BA00-427920F7F315}"/>
   </bookViews>
   <sheets>
     <sheet name="VARIABLES" sheetId="1" r:id="rId1"/>
     <sheet name="Plantilla" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plantilla!$A$1:$AR$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Plantilla!$A$1:$AS$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="423">
   <si>
     <t>Tipo</t>
   </si>
@@ -1300,6 +1300,15 @@
   <si>
     <t xml:space="preserve">DOCENCIA SUPERIOR PSICOLOGÍA (TULCÁN)
 </t>
+  </si>
+  <si>
+    <t>Sede</t>
+  </si>
+  <si>
+    <t>Ibarra</t>
+  </si>
+  <si>
+    <t>Tulcán</t>
   </si>
 </sst>
 </file>
@@ -1509,12 +1518,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1522,6 +1525,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1882,15 +1891,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5126F865-1C20-4858-BFE7-599BE77F5283}">
-  <dimension ref="A1:H302"/>
+  <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1900,8 +1909,11 @@
       <c r="G1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1920,8 +1932,11 @@
       <c r="H2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1940,8 +1955,11 @@
       <c r="H3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1961,7 +1979,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1981,7 +1999,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G6">
         <v>4</v>
       </c>
@@ -1989,7 +2007,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1997,7 +2015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -2005,7 +2023,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2013,7 +2031,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2021,7 +2039,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2029,7 +2047,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -2037,7 +2055,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2045,7 +2063,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -2053,7 +2071,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -3771,17 +3789,17 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="YNIgBKmOCwkYvytKDKgtIlDTDXPRn3vtEgPe505MSL7cr54zUbxq2b7jmEeJob2oev9bcINLJXAOCGwPesPXwA==" saltValue="0GQ1xrpmv7oh1FoIJgD1XA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="H6JmGREBufTP5LP8w66z42N43GmyTx04CF7YQKMELWAxfL6dyTitZ1pst/HFTXhbpcuIAAwAckchE99YwY/W2w==" saltValue="p/3mDrJ0jWUau6R0OkWU+w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4683D6-9C67-4501-B159-2EFC9AEBA871}">
-  <dimension ref="A1:AR3"/>
+  <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+    <sheetView topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AS4" sqref="AS4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3789,27 +3807,27 @@
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:45" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="16"/>
@@ -3824,8 +3842,8 @@
       <c r="R1" s="16"/>
       <c r="S1" s="16"/>
       <c r="T1" s="16"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="5" t="s">
+      <c r="U1" s="9"/>
+      <c r="V1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="W1" s="16"/>
@@ -3846,21 +3864,24 @@
       <c r="AL1" s="16"/>
       <c r="AM1" s="16"/>
       <c r="AN1" s="16"/>
-      <c r="AO1" s="6"/>
+      <c r="AO1" s="9"/>
       <c r="AP1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="AQ1" s="18"/>
-      <c r="AR1" s="7" t="s">
+      <c r="AR1" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:44" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="AS1" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="10" t="s">
         <v>10</v>
       </c>
@@ -3937,14 +3958,15 @@
       <c r="AO2" s="13"/>
       <c r="AP2" s="19"/>
       <c r="AQ2" s="20"/>
-      <c r="AR2" s="8"/>
-    </row>
-    <row r="3" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="AR2" s="6"/>
+      <c r="AS2" s="6"/>
+    </row>
+    <row r="3" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="2" t="s">
@@ -4055,10 +4077,11 @@
       <c r="AQ3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AR3" s="9"/>
+      <c r="AR3" s="7"/>
+      <c r="AS3" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AR3" xr:uid="{4D4683D6-9C67-4501-B159-2EFC9AEBA871}">
+  <autoFilter ref="A1:AS3" xr:uid="{4D4683D6-9C67-4501-B159-2EFC9AEBA871}">
     <filterColumn colId="5" showButton="0"/>
     <filterColumn colId="7" showButton="0"/>
     <filterColumn colId="8" showButton="0"/>
@@ -4094,8 +4117,7 @@
     <filterColumn colId="39" showButton="0"/>
     <filterColumn colId="41" showButton="0"/>
   </autoFilter>
-  <mergeCells count="29">
-    <mergeCell ref="AP1:AQ2"/>
+  <mergeCells count="30">
     <mergeCell ref="AR1:AR3"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
@@ -4110,12 +4132,7 @@
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="AJ2:AK2"/>
     <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="H1:U1"/>
-    <mergeCell ref="V1:AO1"/>
+    <mergeCell ref="AS1:AS3"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
@@ -4124,6 +4141,13 @@
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="H1:U1"/>
+    <mergeCell ref="V1:AO1"/>
+    <mergeCell ref="AP1:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -4133,7 +4157,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6C5A0DE8-8E1F-4568-93A2-C832EE9C40A0}">
           <x14:formula1>
             <xm:f>VARIABLES!$B$3:$B$5</xm:f>
@@ -4164,6 +4188,12 @@
           </x14:formula1>
           <xm:sqref>E4:E1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21ACC545-47AF-47B0-AB18-7CC097D442D7}">
+          <x14:formula1>
+            <xm:f>VARIABLES!$L$2:$L$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>AS4:AS1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
subida por cvs completada
</commit_message>
<xml_diff>
--- a/public/files/csv/plantilla.xlsx
+++ b/public/files/csv/plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XAMPP\htdocs\SistemaGestionDocumental\public\files\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E6DE49-A7EC-48F2-B7A1-BEAE6E9931A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7494978-6E13-4541-B754-1D97F6A48910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E1F0702F-A2B5-47DB-BA00-427920F7F315}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{E1F0702F-A2B5-47DB-BA00-427920F7F315}"/>
   </bookViews>
   <sheets>
     <sheet name="VARIABLES" sheetId="1" r:id="rId1"/>
@@ -1305,10 +1305,10 @@
     <t>Sede</t>
   </si>
   <si>
-    <t>Ibarra</t>
-  </si>
-  <si>
-    <t>Tulcán</t>
+    <t xml:space="preserve">ibarra </t>
+  </si>
+  <si>
+    <t>tulcan</t>
   </si>
 </sst>
 </file>
@@ -1527,6 +1527,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1537,18 +1549,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1891,15 +1891,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5126F865-1C20-4858-BFE7-599BE77F5283}">
-  <dimension ref="A1:L302"/>
+  <dimension ref="A1:M302"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1932,11 +1932,14 @@
       <c r="H2" t="s">
         <v>42</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1955,11 +1958,14 @@
       <c r="H3" t="s">
         <v>43</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1999,7 +2005,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G6">
         <v>4</v>
       </c>
@@ -2007,7 +2013,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2015,7 +2021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -2023,7 +2029,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2039,7 +2045,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2047,7 +2053,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -2055,7 +2061,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2063,7 +2069,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -2071,7 +2077,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -3789,7 +3795,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="H6JmGREBufTP5LP8w66z42N43GmyTx04CF7YQKMELWAxfL6dyTitZ1pst/HFTXhbpcuIAAwAckchE99YwY/W2w==" saltValue="p/3mDrJ0jWUau6R0OkWU+w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3798,8 +3803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4683D6-9C67-4501-B159-2EFC9AEBA871}">
   <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AS4" sqref="AS4"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3823,11 +3828,11 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="16"/>
@@ -3842,8 +3847,8 @@
       <c r="R1" s="16"/>
       <c r="S1" s="16"/>
       <c r="T1" s="16"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="8" t="s">
+      <c r="U1" s="13"/>
+      <c r="V1" s="12" t="s">
         <v>7</v>
       </c>
       <c r="W1" s="16"/>
@@ -3864,7 +3869,7 @@
       <c r="AL1" s="16"/>
       <c r="AM1" s="16"/>
       <c r="AN1" s="16"/>
-      <c r="AO1" s="9"/>
+      <c r="AO1" s="13"/>
       <c r="AP1" s="17" t="s">
         <v>8</v>
       </c>
@@ -3882,80 +3887,80 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="12" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="12" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="12" t="s">
+      <c r="M2" s="9"/>
+      <c r="N2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="12" t="s">
+      <c r="O2" s="9"/>
+      <c r="P2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="12" t="s">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="12" t="s">
+      <c r="S2" s="9"/>
+      <c r="T2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="13"/>
-      <c r="V2" s="12" t="s">
+      <c r="U2" s="9"/>
+      <c r="V2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="13"/>
-      <c r="X2" s="12" t="s">
+      <c r="W2" s="9"/>
+      <c r="X2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="14" t="s">
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="14" t="s">
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="12" t="s">
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="12" t="s">
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AG2" s="13"/>
-      <c r="AH2" s="12" t="s">
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="12" t="s">
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AK2" s="13"/>
-      <c r="AL2" s="12" t="s">
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AM2" s="13"/>
-      <c r="AN2" s="12" t="s">
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AO2" s="13"/>
+      <c r="AO2" s="9"/>
       <c r="AP2" s="19"/>
       <c r="AQ2" s="20"/>
       <c r="AR2" s="6"/>
@@ -3967,8 +3972,8 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
@@ -4118,20 +4123,6 @@
     <filterColumn colId="41" showButton="0"/>
   </autoFilter>
   <mergeCells count="30">
-    <mergeCell ref="AR1:AR3"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
     <mergeCell ref="AS1:AS3"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="A1:A3"/>
@@ -4148,6 +4139,20 @@
     <mergeCell ref="H1:U1"/>
     <mergeCell ref="V1:AO1"/>
     <mergeCell ref="AP1:AQ2"/>
+    <mergeCell ref="AR1:AR3"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>